<commit_message>
Add new session 28-07-23
</commit_message>
<xml_diff>
--- a/Doubles training.xlsx
+++ b/Doubles training.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1046,6 +1046,168 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>246077</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2023-07-21T15:19:19.000000Z</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="n">
+        <v>23</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
+      <c r="I8" t="n">
+        <v>30</v>
+      </c>
+      <c r="J8" t="n">
+        <v>8</v>
+      </c>
+      <c r="K8" t="n">
+        <v>14</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4</v>
+      </c>
+      <c r="N8" t="n">
+        <v>11</v>
+      </c>
+      <c r="O8" t="n">
+        <v>3</v>
+      </c>
+      <c r="P8" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>21</v>
+      </c>
+      <c r="R8" t="n">
+        <v>3</v>
+      </c>
+      <c r="S8" t="n">
+        <v>10</v>
+      </c>
+      <c r="T8" t="n">
+        <v>15</v>
+      </c>
+      <c r="U8" t="n">
+        <v>14</v>
+      </c>
+      <c r="V8" t="n">
+        <v>2</v>
+      </c>
+      <c r="W8" t="n">
+        <v>6</v>
+      </c>
+      <c r="X8" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>248429</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2023-07-28T18:38:43.000000Z</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="E9" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19</v>
+      </c>
+      <c r="J9" t="n">
+        <v>3</v>
+      </c>
+      <c r="K9" t="n">
+        <v>17</v>
+      </c>
+      <c r="L9" t="n">
+        <v>13</v>
+      </c>
+      <c r="M9" t="n">
+        <v>17</v>
+      </c>
+      <c r="N9" t="n">
+        <v>16</v>
+      </c>
+      <c r="O9" t="n">
+        <v>15</v>
+      </c>
+      <c r="P9" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
+        <v>6</v>
+      </c>
+      <c r="S9" t="n">
+        <v>2</v>
+      </c>
+      <c r="T9" t="n">
+        <v>5</v>
+      </c>
+      <c r="U9" t="n">
+        <v>23</v>
+      </c>
+      <c r="V9" t="n">
+        <v>19</v>
+      </c>
+      <c r="W9" t="n">
+        <v>22</v>
+      </c>
+      <c r="X9" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>